<commit_message>
docs: add Maquette.png and update MCD and Rbac
</commit_message>
<xml_diff>
--- a/docs/Rbac.xlsx
+++ b/docs/Rbac.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="24">
   <si>
     <t>Client</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>accès à la page de gestion des avis</t>
+  </si>
+  <si>
+    <t>accès à la page de gestion des commande</t>
   </si>
 </sst>
 </file>
@@ -416,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,6 +706,17 @@
         <v>19</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>